<commit_message>
#17 Fixed job title, company name, location and summary in indeed
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1" refMode="A1" iterate="0" iterateCount="100" iterateDelta="0.001"/>
@@ -465,7 +465,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F38"/>
+  <dimension ref="A1:F41"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -508,7 +508,7 @@
     <row r="2">
       <c r="A2" s="0" t="inlineStr">
         <is>
-          <t>Web Developer</t>
+          <t>FULL STACK DEVELOPER</t>
         </is>
       </c>
       <c r="B2" s="0" t="inlineStr"/>
@@ -518,21 +518,17 @@
         </is>
       </c>
       <c r="D2" s="0" t="inlineStr"/>
-      <c r="E2" s="0" t="inlineStr">
-        <is>
-          <t>5 days ago</t>
-        </is>
-      </c>
+      <c r="E2" s="0" t="inlineStr"/>
       <c r="F2" s="0" t="inlineStr">
         <is>
-          <t>https://ae.linkedin.com/jobs/view/web-developer-at-creative-zone-2613193658?refId=KDMiu2nd26KwBGPnJcFktg%3D%3D&amp;trackingId=O5qabPMf5ZKao0cf1qwXFg%3D%3D&amp;position=1&amp;pageNum=0&amp;trk=public_jobs_jserp-result_search-card</t>
+          <t>https://ae.linkedin.com/jobs/view/full-stack-developer-at-digital-squad-australia-2631931145?refId=ieeFurlekIzfvvNO4EJ7cQ%3D%3D&amp;trackingId=oVl7VpDueCkEzOScurbnPw%3D%3D&amp;position=1&amp;pageNum=0&amp;trk=public_jobs_jserp-result_search-card</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="0" t="inlineStr">
         <is>
-          <t>Web Developer</t>
+          <t>Back End Developer</t>
         </is>
       </c>
       <c r="B3" s="0" t="inlineStr"/>
@@ -544,19 +540,19 @@
       <c r="D3" s="0" t="inlineStr"/>
       <c r="E3" s="0" t="inlineStr">
         <is>
-          <t>4 weeks ago</t>
+          <t>2 days ago</t>
         </is>
       </c>
       <c r="F3" s="0" t="inlineStr">
         <is>
-          <t>https://ae.linkedin.com/jobs/view/web-developer-at-naffco-fzco-2582654452?refId=KDMiu2nd26KwBGPnJcFktg%3D%3D&amp;trackingId=ZcaNvVf6K%2F6qAV%2BaRybQQg%3D%3D&amp;position=2&amp;pageNum=0&amp;trk=public_jobs_jserp-result_search-card</t>
+          <t>https://ae.linkedin.com/jobs/view/back-end-developer-at-aspire-mena-2630813687?refId=ieeFurlekIzfvvNO4EJ7cQ%3D%3D&amp;trackingId=OU52J5JeK010Osxcv7etUg%3D%3D&amp;position=2&amp;pageNum=0&amp;trk=public_jobs_jserp-result_search-card</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="0" t="inlineStr">
         <is>
-          <t>Back End Developer</t>
+          <t>Junior Developer</t>
         </is>
       </c>
       <c r="B4" s="0" t="inlineStr"/>
@@ -568,43 +564,43 @@
       <c r="D4" s="0" t="inlineStr"/>
       <c r="E4" s="0" t="inlineStr">
         <is>
-          <t>1 day ago</t>
+          <t>2 weeks ago</t>
         </is>
       </c>
       <c r="F4" s="0" t="inlineStr">
         <is>
-          <t>https://ae.linkedin.com/jobs/view/back-end-developer-at-agile-consultants-2625815454?refId=KDMiu2nd26KwBGPnJcFktg%3D%3D&amp;trackingId=Td8%2FaHXXiItIfs1WAhy3NA%3D%3D&amp;position=4&amp;pageNum=0&amp;trk=public_jobs_jserp-result_search-card</t>
+          <t>https://ae.linkedin.com/jobs/view/junior-developer-at-chalhoub-group-2609233473?refId=ieeFurlekIzfvvNO4EJ7cQ%3D%3D&amp;trackingId=SgO%2BafoWMuG0woUFrsCTzA%3D%3D&amp;position=3&amp;pageNum=0&amp;trk=public_jobs_jserp-result_search-card</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="0" t="inlineStr">
         <is>
-          <t>Full Stack Developer</t>
+          <t>JUNIOR DEVELOPER - Dubai or Remote</t>
         </is>
       </c>
       <c r="B5" s="0" t="inlineStr"/>
       <c r="C5" s="0" t="inlineStr">
         <is>
-          <t>Dubai, United Arab Emirates</t>
+          <t>Dubai, Dubai, United Arab Emirates</t>
         </is>
       </c>
       <c r="D5" s="0" t="inlineStr"/>
       <c r="E5" s="0" t="inlineStr">
         <is>
-          <t>1 week ago</t>
+          <t>1 month ago</t>
         </is>
       </c>
       <c r="F5" s="0" t="inlineStr">
         <is>
-          <t>https://ae.linkedin.com/jobs/view/full-stack-developer-at-focus-academy-2621312048?refId=KDMiu2nd26KwBGPnJcFktg%3D%3D&amp;trackingId=l6d9rzpT6pssmDDt%2FSWGgw%3D%3D&amp;position=5&amp;pageNum=0&amp;trk=public_jobs_jserp-result_search-card</t>
+          <t>https://ae.linkedin.com/jobs/view/junior-developer-dubai-or-remote-at-cobblestone-energy-2616837676?refId=ieeFurlekIzfvvNO4EJ7cQ%3D%3D&amp;trackingId=AU%2FFt79AUcc2Onkr4IjxgA%3D%3D&amp;position=4&amp;pageNum=0&amp;trk=public_jobs_jserp-result_search-card</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="0" t="inlineStr">
         <is>
-          <t>Développeur back-end - Node.JS</t>
+          <t>Full Stack Engineer</t>
         </is>
       </c>
       <c r="B6" s="0" t="inlineStr"/>
@@ -616,19 +612,19 @@
       <c r="D6" s="0" t="inlineStr"/>
       <c r="E6" s="0" t="inlineStr">
         <is>
-          <t>2 months ago</t>
+          <t>2 weeks ago</t>
         </is>
       </c>
       <c r="F6" s="0" t="inlineStr">
         <is>
-          <t>https://ae.linkedin.com/jobs/view/d%C3%A9veloppeur-back-end-node-js-at-paradox-2532478802?refId=KDMiu2nd26KwBGPnJcFktg%3D%3D&amp;trackingId=cH6xwJB7Dvw22Y8nFFlAWQ%3D%3D&amp;position=7&amp;pageNum=0&amp;trk=public_jobs_jserp-result_search-card</t>
+          <t>https://ae.linkedin.com/jobs/view/full-stack-engineer-at-klanik-2606377905?refId=ieeFurlekIzfvvNO4EJ7cQ%3D%3D&amp;trackingId=6ZH0C3FNCWXt6ipNKfcIVw%3D%3D&amp;position=5&amp;pageNum=0&amp;trk=public_jobs_jserp-result_search-card</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="0" t="inlineStr">
         <is>
-          <t>Portal Development Manager</t>
+          <t>Software Developer</t>
         </is>
       </c>
       <c r="B7" s="0" t="inlineStr"/>
@@ -640,19 +636,19 @@
       <c r="D7" s="0" t="inlineStr"/>
       <c r="E7" s="0" t="inlineStr">
         <is>
-          <t>1 week ago</t>
+          <t>2 days ago</t>
         </is>
       </c>
       <c r="F7" s="0" t="inlineStr">
         <is>
-          <t>https://ae.linkedin.com/jobs/view/portal-development-manager-at-bso-2621306782?refId=KDMiu2nd26KwBGPnJcFktg%3D%3D&amp;trackingId=DB9ZBGPsUSzXf0wPgOsaBg%3D%3D&amp;position=8&amp;pageNum=0&amp;trk=public_jobs_jserp-result_search-card</t>
+          <t>https://ae.linkedin.com/jobs/view/software-developer-at-dun-bradstreet-south-asia-middle-east-ltd-2630836245?refId=ieeFurlekIzfvvNO4EJ7cQ%3D%3D&amp;trackingId=Za7Bhy6z%2FbOowdGlCtBbrQ%3D%3D&amp;position=6&amp;pageNum=0&amp;trk=public_jobs_jserp-result_search-card</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="0" t="inlineStr">
         <is>
-          <t>Magento Developer</t>
+          <t>Front End Developer</t>
         </is>
       </c>
       <c r="B8" s="0" t="inlineStr"/>
@@ -664,19 +660,19 @@
       <c r="D8" s="0" t="inlineStr"/>
       <c r="E8" s="0" t="inlineStr">
         <is>
-          <t>4 weeks ago</t>
+          <t>1 week ago</t>
         </is>
       </c>
       <c r="F8" s="0" t="inlineStr">
         <is>
-          <t>https://ae.linkedin.com/jobs/view/magento-developer-at-groupe-rhinos-2584110169?refId=KDMiu2nd26KwBGPnJcFktg%3D%3D&amp;trackingId=JMOPIJbZ6bgAzthl79BZEQ%3D%3D&amp;position=9&amp;pageNum=0&amp;trk=public_jobs_jserp-result_search-card</t>
+          <t>https://ae.linkedin.com/jobs/view/front-end-developer-at-%D8%AF%D8%A8%D9%8A-%D8%A7%D9%84%D8%B0%D9%83%D9%8A%D8%A9-2615996415?refId=ieeFurlekIzfvvNO4EJ7cQ%3D%3D&amp;trackingId=UvrJ0lt74YuE3HEMw4tnWQ%3D%3D&amp;position=7&amp;pageNum=0&amp;trk=public_jobs_jserp-result_search-card</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="0" t="inlineStr">
         <is>
-          <t>Tech Lead aspiring Engineering Manager</t>
+          <t>Full Stack Developer</t>
         </is>
       </c>
       <c r="B9" s="0" t="inlineStr"/>
@@ -688,84 +684,116 @@
       <c r="D9" s="0" t="inlineStr"/>
       <c r="E9" s="0" t="inlineStr">
         <is>
-          <t>2 months ago</t>
+          <t>3 weeks ago</t>
         </is>
       </c>
       <c r="F9" s="0" t="inlineStr">
         <is>
-          <t>https://ae.linkedin.com/jobs/view/tech-lead-aspiring-engineering-manager-at-paradox-2540758527?refId=KDMiu2nd26KwBGPnJcFktg%3D%3D&amp;trackingId=%2BI5BIO0KSInuw7x1Hsie%2Bw%3D%3D&amp;position=10&amp;pageNum=0&amp;trk=public_jobs_jserp-result_search-card</t>
+          <t>https://ae.linkedin.com/jobs/view/full-stack-developer-at-ntamtech-2598020783?refId=ieeFurlekIzfvvNO4EJ7cQ%3D%3D&amp;trackingId=z9GW1ake7%2BVvhelAAJEICw%3D%3D&amp;position=8&amp;pageNum=0&amp;trk=public_jobs_jserp-result_search-card</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="0" t="inlineStr">
         <is>
-          <t>Senior PHP Developer - Laravel / MySQL</t>
+          <t>Full Stack Developer</t>
         </is>
       </c>
       <c r="B10" s="0" t="inlineStr"/>
-      <c r="C10" s="0" t="inlineStr"/>
+      <c r="C10" s="0" t="inlineStr">
+        <is>
+          <t>Dubai, United Arab Emirates</t>
+        </is>
+      </c>
       <c r="D10" s="0" t="inlineStr"/>
       <c r="E10" s="0" t="inlineStr">
         <is>
-          <t>30+ days ago</t>
+          <t>3 weeks ago</t>
         </is>
       </c>
       <c r="F10" s="0" t="inlineStr">
         <is>
-          <t>https://ae.indeed.com/rc/clk?jk=b721c367fb7f4e05&amp;fccid=71590b46c05f8c89&amp;vjs=3</t>
+          <t>https://ae.linkedin.com/jobs/view/full-stack-developer-at-creative-technology-solution-2596737192?refId=ieeFurlekIzfvvNO4EJ7cQ%3D%3D&amp;trackingId=AgMHR2VQZArdKAl4Fukt9A%3D%3D&amp;position=9&amp;pageNum=0&amp;trk=public_jobs_jserp-result_search-card</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="0" t="inlineStr">
         <is>
-          <t>PHP Developer</t>
+          <t>Back End Developer</t>
         </is>
       </c>
       <c r="B11" s="0" t="inlineStr"/>
-      <c r="C11" s="0" t="inlineStr"/>
+      <c r="C11" s="0" t="inlineStr">
+        <is>
+          <t>Dubai, United Arab Emirates</t>
+        </is>
+      </c>
       <c r="D11" s="0" t="inlineStr"/>
       <c r="E11" s="0" t="inlineStr">
         <is>
-          <t>30+ days ago</t>
+          <t>3 weeks ago</t>
         </is>
       </c>
       <c r="F11" s="0" t="inlineStr">
         <is>
-          <t>https://ae.indeed.com/rc/clk?jk=6dab182edd88b96f&amp;fccid=a4a6d84f02499146&amp;vjs=3</t>
+          <t>https://ae.linkedin.com/jobs/view/back-end-developer-at-iown-group-2594607107?refId=ieeFurlekIzfvvNO4EJ7cQ%3D%3D&amp;trackingId=1sv2zVDrmLU%2FTw3OWiU9Ig%3D%3D&amp;position=10&amp;pageNum=0&amp;trk=public_jobs_jserp-result_search-card</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="0" t="inlineStr">
         <is>
-          <t>We are seeking a Full Stack Developer with SaaS experience.</t>
-        </is>
-      </c>
-      <c r="B12" s="0" t="inlineStr"/>
-      <c r="C12" s="0" t="inlineStr"/>
-      <c r="D12" s="0" t="inlineStr"/>
+          <t>Junior Developer</t>
+        </is>
+      </c>
+      <c r="B12" s="0" t="inlineStr">
+        <is>
+          <t>Chalhoub Group</t>
+        </is>
+      </c>
+      <c r="C12" s="0" t="inlineStr">
+        <is>
+          <t>Dubai</t>
+        </is>
+      </c>
+      <c r="D12" s="0" t="inlineStr">
+        <is>
+          <t>Our Junior Developer will have a passion for digital learning technology and education.</t>
+        </is>
+      </c>
       <c r="E12" s="0" t="inlineStr">
         <is>
-          <t>30+ days ago</t>
+          <t>13 days ago</t>
         </is>
       </c>
       <c r="F12" s="0" t="inlineStr">
         <is>
-          <t>https://ae.indeed.com/rc/clk?jk=35380171cff2f957&amp;fccid=7021cc13a0d80157&amp;vjs=3</t>
+          <t>https://ae.indeed.com/rc/clk?jk=1ba5d39196e907f5&amp;fccid=01f47b3f00b281a4&amp;vjs=3</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="0" t="inlineStr">
         <is>
-          <t>Back-end Developer</t>
-        </is>
-      </c>
-      <c r="B13" s="0" t="inlineStr"/>
-      <c r="C13" s="0" t="inlineStr"/>
-      <c r="D13" s="0" t="inlineStr"/>
+          <t>IT Technician</t>
+        </is>
+      </c>
+      <c r="B13" s="0" t="inlineStr">
+        <is>
+          <t>Scientific Analytical Tools</t>
+        </is>
+      </c>
+      <c r="C13" s="0" t="inlineStr">
+        <is>
+          <t>Dubai</t>
+        </is>
+      </c>
+      <c r="D13" s="0" t="inlineStr">
+        <is>
+          <t>Rapidly establishing a good working relationship with customers and other professionals, such as software developers;</t>
+        </is>
+      </c>
       <c r="E13" s="0" t="inlineStr">
         <is>
           <t>30+ days ago</t>
@@ -773,19 +801,31 @@
       </c>
       <c r="F13" s="0" t="inlineStr">
         <is>
-          <t>https://ae.indeed.com/rc/clk?jk=96ed662a940490b1&amp;fccid=559e98f2d4dfbf56&amp;vjs=3</t>
+          <t>https://ae.indeed.com/rc/clk?jk=f58903c3e48a9286&amp;fccid=0e0b320a90f3822f&amp;vjs=3</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="0" t="inlineStr">
         <is>
-          <t>PHP Developer</t>
-        </is>
-      </c>
-      <c r="B14" s="0" t="inlineStr"/>
-      <c r="C14" s="0" t="inlineStr"/>
-      <c r="D14" s="0" t="inlineStr"/>
+          <t>Junior Software Developer</t>
+        </is>
+      </c>
+      <c r="B14" s="0" t="inlineStr">
+        <is>
+          <t>Dotcom Systems</t>
+        </is>
+      </c>
+      <c r="C14" s="0" t="inlineStr">
+        <is>
+          <t>Dubai</t>
+        </is>
+      </c>
+      <c r="D14" s="0" t="inlineStr">
+        <is>
+          <t>C#, VB.net, SQL, Crystal Reports, HTML5, ASP.net, Android, SQL Lite.</t>
+        </is>
+      </c>
       <c r="E14" s="0" t="inlineStr">
         <is>
           <t>30+ days ago</t>
@@ -793,34 +833,63 @@
       </c>
       <c r="F14" s="0" t="inlineStr">
         <is>
-          <t>https://ae.indeed.com/rc/clk?jk=ba93b8dce75a73af&amp;fccid=c84d6205b9d4151d&amp;vjs=3</t>
+          <t>https://ae.indeed.com/rc/clk?jk=b6ba5c262223cdb6&amp;fccid=a6e9af6552e4f905&amp;vjs=3</t>
         </is>
       </c>
     </row>
     <row r="15">
-      <c r="B15" s="0" t="inlineStr"/>
-      <c r="C15" s="0" t="inlineStr"/>
-      <c r="D15" s="0" t="inlineStr"/>
+      <c r="A15" s="0" t="inlineStr">
+        <is>
+          <t>Web and It Support</t>
+        </is>
+      </c>
+      <c r="B15" s="0" t="inlineStr">
+        <is>
+          <t>PRO Consult</t>
+        </is>
+      </c>
+      <c r="C15" s="0" t="inlineStr">
+        <is>
+          <t>Dubai</t>
+        </is>
+      </c>
+      <c r="D15" s="0" t="inlineStr">
+        <is>
+          <t>As a Web and IT Support, you will be responsible for company’s website and providing all support related to IT, Computer hardware and Softwares.</t>
+        </is>
+      </c>
       <c r="E15" s="0" t="inlineStr">
         <is>
-          <t>4 days ago</t>
+          <t>30+ days ago</t>
         </is>
       </c>
       <c r="F15" s="0" t="inlineStr">
         <is>
-          <t>https://ae.indeed.com/rc/clk?jk=a6460e293343a1c7&amp;fccid=a0f4df2b71213d85&amp;vjs=3</t>
+          <t>https://ae.indeed.com/rc/clk?jk=f3c3abecadea8597&amp;fccid=55c333e3bcc1820f&amp;vjs=3</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="0" t="inlineStr">
         <is>
-          <t>Drupal/Wordpress PHP Developer</t>
-        </is>
-      </c>
-      <c r="B16" s="0" t="inlineStr"/>
-      <c r="C16" s="0" t="inlineStr"/>
-      <c r="D16" s="0" t="inlineStr"/>
+          <t>Back-end Developer</t>
+        </is>
+      </c>
+      <c r="B16" s="0" t="inlineStr">
+        <is>
+          <t>TenTwenty</t>
+        </is>
+      </c>
+      <c r="C16" s="0" t="inlineStr">
+        <is>
+          <t>Dubai</t>
+        </is>
+      </c>
+      <c r="D16" s="0" t="inlineStr">
+        <is>
+          <t>Smart working developer with an eye for detail and following the coding standards.</t>
+        </is>
+      </c>
       <c r="E16" s="0" t="inlineStr">
         <is>
           <t>30+ days ago</t>
@@ -828,74 +897,127 @@
       </c>
       <c r="F16" s="0" t="inlineStr">
         <is>
-          <t>https://ae.indeed.com/rc/clk?jk=0e953b5b01639b87&amp;fccid=01fa4c4529403dd7&amp;vjs=3</t>
+          <t>https://ae.indeed.com/rc/clk?jk=96ed662a940490b1&amp;fccid=559e98f2d4dfbf56&amp;vjs=3</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="0" t="inlineStr">
         <is>
-          <t>Software Development Lead</t>
-        </is>
-      </c>
-      <c r="B17" s="0" t="inlineStr"/>
-      <c r="C17" s="0" t="inlineStr"/>
-      <c r="D17" s="0" t="inlineStr"/>
+          <t>React Native Developer</t>
+        </is>
+      </c>
+      <c r="B17" s="0" t="inlineStr">
+        <is>
+          <t>ECS ME LLC</t>
+        </is>
+      </c>
+      <c r="C17" s="0" t="inlineStr">
+        <is>
+          <t>Dubai</t>
+        </is>
+      </c>
+      <c r="D17" s="0" t="inlineStr">
+        <is>
+          <t>We are looking for a React Native developer (with 4-5 Yrs of work exp.).</t>
+        </is>
+      </c>
       <c r="E17" s="0" t="inlineStr">
         <is>
-          <t>30+ days ago</t>
+          <t>6 days ago</t>
         </is>
       </c>
       <c r="F17" s="0" t="inlineStr">
         <is>
-          <t>https://ae.indeed.com/rc/clk?jk=771aa13ce046c153&amp;fccid=ca393fdec5169bcb&amp;vjs=3</t>
+          <t>https://ae.indeed.com/company/ECS-ME-LLC/jobs/React-Native-Developer-2edd107ea5c703fa?fccid=d99f94aeddf34dc7&amp;vjs=3</t>
         </is>
       </c>
     </row>
     <row r="18">
-      <c r="B18" s="0" t="inlineStr"/>
-      <c r="C18" s="0" t="inlineStr"/>
-      <c r="D18" s="0" t="inlineStr"/>
+      <c r="A18" s="0" t="inlineStr">
+        <is>
+          <t>Front-end Developer</t>
+        </is>
+      </c>
+      <c r="B18" s="0" t="inlineStr">
+        <is>
+          <t>TenTwenty</t>
+        </is>
+      </c>
+      <c r="C18" s="0" t="inlineStr">
+        <is>
+          <t>Dubai</t>
+        </is>
+      </c>
+      <c r="D18" s="0" t="inlineStr">
+        <is>
+          <t>Basic understanding of Sketch and creating assets for the front-end development.</t>
+        </is>
+      </c>
       <c r="E18" s="0" t="inlineStr">
         <is>
-          <t>5 days ago</t>
+          <t>30+ days ago</t>
         </is>
       </c>
       <c r="F18" s="0" t="inlineStr">
         <is>
-          <t>https://ae.indeed.com/rc/clk?jk=aad8334ceccc416e&amp;fccid=92e5bc1ee7cc479a&amp;vjs=3</t>
+          <t>https://ae.indeed.com/rc/clk?jk=121fb3259e880115&amp;fccid=559e98f2d4dfbf56&amp;vjs=3</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="0" t="inlineStr">
         <is>
-          <t>Full Stack Web Developer</t>
-        </is>
-      </c>
-      <c r="B19" s="0" t="inlineStr"/>
-      <c r="C19" s="0" t="inlineStr"/>
-      <c r="D19" s="0" t="inlineStr"/>
+          <t>Software Developer Trainee (India)</t>
+        </is>
+      </c>
+      <c r="B19" s="0" t="inlineStr">
+        <is>
+          <t>Metadata</t>
+        </is>
+      </c>
+      <c r="C19" s="0" t="inlineStr">
+        <is>
+          <t>Dubai</t>
+        </is>
+      </c>
+      <c r="D19" s="0" t="inlineStr">
+        <is>
+          <t>Need to have basic ASP.</t>
+        </is>
+      </c>
       <c r="E19" s="0" t="inlineStr">
         <is>
-          <t>28 days ago</t>
+          <t>30+ days ago</t>
         </is>
       </c>
       <c r="F19" s="0" t="inlineStr">
         <is>
-          <t>https://ae.indeed.com/rc/clk?jk=1817d6b717aa4758&amp;fccid=2e446275f8cd19d2&amp;vjs=3</t>
+          <t>https://ae.indeed.com/rc/clk?jk=07e1a7df822e3846&amp;fccid=6c72041b951272af&amp;vjs=3</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="0" t="inlineStr">
         <is>
-          <t>Full Stack Web Developer</t>
-        </is>
-      </c>
-      <c r="B20" s="0" t="inlineStr"/>
-      <c r="C20" s="0" t="inlineStr"/>
-      <c r="D20" s="0" t="inlineStr"/>
+          <t>Oracle Developer</t>
+        </is>
+      </c>
+      <c r="B20" s="0" t="inlineStr">
+        <is>
+          <t>Emirates Driving Institute (EDI)</t>
+        </is>
+      </c>
+      <c r="C20" s="0" t="inlineStr">
+        <is>
+          <t>Dubai</t>
+        </is>
+      </c>
+      <c r="D20" s="0" t="inlineStr">
+        <is>
+          <t>Minimum 4 years of experience in writing &amp; turning Oracle SQL and PL/SQL.</t>
+        </is>
+      </c>
       <c r="E20" s="0" t="inlineStr">
         <is>
           <t>30+ days ago</t>
@@ -903,84 +1025,159 @@
       </c>
       <c r="F20" s="0" t="inlineStr">
         <is>
-          <t>https://ae.indeed.com/rc/clk?jk=dd3bea9ff4bbfdd8&amp;fccid=144ad60e18d268b0&amp;vjs=3</t>
+          <t>https://ae.indeed.com/rc/clk?jk=2a37a183702d4de3&amp;fccid=b3180e8cd43ce258&amp;vjs=3</t>
         </is>
       </c>
     </row>
     <row r="21">
-      <c r="B21" s="0" t="inlineStr"/>
-      <c r="C21" s="0" t="inlineStr"/>
-      <c r="D21" s="0" t="inlineStr"/>
+      <c r="A21" s="0" t="inlineStr">
+        <is>
+          <t>Backend Developer - UAE</t>
+        </is>
+      </c>
+      <c r="B21" s="0" t="inlineStr">
+        <is>
+          <t>Snowfall</t>
+        </is>
+      </c>
+      <c r="C21" s="0" t="inlineStr">
+        <is>
+          <t>Dubai</t>
+        </is>
+      </c>
+      <c r="D21" s="0" t="inlineStr">
+        <is>
+          <t>Mentor and coach other backend developers within the team.</t>
+        </is>
+      </c>
       <c r="E21" s="0" t="inlineStr">
         <is>
-          <t>7 days ago</t>
+          <t>4 days ago</t>
         </is>
       </c>
       <c r="F21" s="0" t="inlineStr">
         <is>
-          <t>https://ae.indeed.com/company/Transportr.com/jobs/Full-Stack-Developer-e3cc165a86a49931?fccid=4798e1ba3ba0d986&amp;vjs=3</t>
+          <t>https://ae.indeed.com/rc/clk?jk=635918f81ffcfe00&amp;fccid=481367240ce1ecca&amp;vjs=3</t>
         </is>
       </c>
     </row>
     <row r="22">
-      <c r="B22" s="0" t="inlineStr"/>
-      <c r="C22" s="0" t="inlineStr"/>
-      <c r="D22" s="0" t="inlineStr"/>
+      <c r="A22" s="0" t="inlineStr">
+        <is>
+          <t>front-end developer</t>
+        </is>
+      </c>
+      <c r="B22" s="0" t="inlineStr">
+        <is>
+          <t>PSdigital</t>
+        </is>
+      </c>
+      <c r="C22" s="0" t="inlineStr">
+        <is>
+          <t>Dubai</t>
+        </is>
+      </c>
+      <c r="D22" s="0" t="inlineStr">
+        <is>
+          <t>Collaborate and Support with Back-end developers and Solve problems.</t>
+        </is>
+      </c>
       <c r="E22" s="0" t="inlineStr">
         <is>
-          <t>Just posted</t>
+          <t>30+ days ago</t>
         </is>
       </c>
       <c r="F22" s="0" t="inlineStr">
         <is>
-          <t>https://ae.indeed.com/company/Resource-Log-LLC/jobs/Full-Stack-Developer-f467f8844a454ac3?fccid=415cd241779a8615&amp;vjs=3</t>
+          <t>https://ae.indeed.com/rc/clk?jk=4db438e90c517437&amp;fccid=2f136e3ccf030f0e&amp;vjs=3</t>
         </is>
       </c>
     </row>
     <row r="23">
-      <c r="B23" s="0" t="inlineStr"/>
-      <c r="C23" s="0" t="inlineStr"/>
-      <c r="D23" s="0" t="inlineStr"/>
+      <c r="A23" s="0" t="inlineStr">
+        <is>
+          <t>Microsoft DotNet Developer</t>
+        </is>
+      </c>
+      <c r="B23" s="0" t="inlineStr">
+        <is>
+          <t>eVision IT Solution</t>
+        </is>
+      </c>
+      <c r="C23" s="0" t="inlineStr">
+        <is>
+          <t>Dubai</t>
+        </is>
+      </c>
+      <c r="D23" s="0" t="inlineStr">
+        <is>
+          <t>Net developer responsible for building applications.</t>
+        </is>
+      </c>
       <c r="E23" s="0" t="inlineStr">
         <is>
-          <t>1 day ago</t>
+          <t>30+ days ago</t>
         </is>
       </c>
       <c r="F23" s="0" t="inlineStr">
         <is>
-          <t>https://ae.indeed.com/company/InkMASH/jobs/Full-Stack-PHP-Developer-Strong-Laravel-API-Experience-909cfa0ca3e9e834?fccid=af177f7006244e87&amp;vjs=3</t>
+          <t>https://ae.indeed.com/rc/clk?jk=7cfdf7f87f405610&amp;fccid=a67dd580ec839de8&amp;vjs=3</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="0" t="inlineStr">
         <is>
-          <t>Senior Backend Developer</t>
-        </is>
-      </c>
-      <c r="B24" s="0" t="inlineStr"/>
-      <c r="C24" s="0" t="inlineStr"/>
-      <c r="D24" s="0" t="inlineStr"/>
+          <t>Node JS Developer</t>
+        </is>
+      </c>
+      <c r="B24" s="0" t="inlineStr">
+        <is>
+          <t>Raqmiyat</t>
+        </is>
+      </c>
+      <c r="C24" s="0" t="inlineStr">
+        <is>
+          <t>Dubai</t>
+        </is>
+      </c>
+      <c r="D24" s="0" t="inlineStr">
+        <is>
+          <t>Strong understanding of JavaScript/Object-Oriented JS, its quirks, and workarounds • Must have a working knowledge of Node JS • Must know anyone Node JS…</t>
+        </is>
+      </c>
       <c r="E24" s="0" t="inlineStr">
         <is>
-          <t>26 days ago</t>
+          <t>27 days ago</t>
         </is>
       </c>
       <c r="F24" s="0" t="inlineStr">
         <is>
-          <t>https://ae.indeed.com/company/Shaadoow-Web-Design/jobs/Senior-Backend-Developer-2fc610e35573eae7?fccid=3050515fb97c8120&amp;vjs=3</t>
+          <t>https://ae.indeed.com/rc/clk?jk=aff4b6fde4b96da1&amp;fccid=7afa5fdaf37013fe&amp;vjs=3</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="0" t="inlineStr">
         <is>
-          <t>Back-end Developer (PHP/Laravel/Node.JS/Python)</t>
-        </is>
-      </c>
-      <c r="B25" s="0" t="inlineStr"/>
-      <c r="C25" s="0" t="inlineStr"/>
-      <c r="D25" s="0" t="inlineStr"/>
+          <t>Sr. Andorid Developer</t>
+        </is>
+      </c>
+      <c r="B25" s="0" t="inlineStr">
+        <is>
+          <t>Pegasus</t>
+        </is>
+      </c>
+      <c r="C25" s="0" t="inlineStr">
+        <is>
+          <t>Dubai</t>
+        </is>
+      </c>
+      <c r="D25" s="0" t="inlineStr">
+        <is>
+          <t>We offer a full range of professional service to retailers.</t>
+        </is>
+      </c>
       <c r="E25" s="0" t="inlineStr">
         <is>
           <t>30+ days ago</t>
@@ -988,114 +1185,223 @@
       </c>
       <c r="F25" s="0" t="inlineStr">
         <is>
-          <t>https://ae.indeed.com/company/Resource-Log-LLC/jobs/Back-End-Developer-4b99383b3a27e02f?fccid=415cd241779a8615&amp;vjs=3</t>
+          <t>https://ae.indeed.com/rc/clk?jk=63cbb8c6572845d6&amp;fccid=24491e08f76aeae2&amp;vjs=3</t>
         </is>
       </c>
     </row>
     <row r="26">
-      <c r="B26" s="0" t="inlineStr"/>
-      <c r="C26" s="0" t="inlineStr"/>
-      <c r="D26" s="0" t="inlineStr"/>
+      <c r="A26" s="0" t="inlineStr">
+        <is>
+          <t>Software Developer</t>
+        </is>
+      </c>
+      <c r="B26" s="0" t="inlineStr">
+        <is>
+          <t>Scientific Analytical Tools</t>
+        </is>
+      </c>
+      <c r="C26" s="0" t="inlineStr">
+        <is>
+          <t>Dubai</t>
+        </is>
+      </c>
+      <c r="D26" s="0" t="inlineStr">
+        <is>
+          <t>Work with API developers across the teams to Design/build new API features at large-scale.</t>
+        </is>
+      </c>
       <c r="E26" s="0" t="inlineStr">
         <is>
-          <t>8 days ago</t>
+          <t>30+ days ago</t>
         </is>
       </c>
       <c r="F26" s="0" t="inlineStr">
         <is>
-          <t>https://ae.indeed.com/company/Brainstorm-Human-Resources-Consultants/jobs/Web-Developer-701a0e37d5f1fe4d?fccid=b0bc31d2ce72d680&amp;vjs=3</t>
+          <t>https://ae.indeed.com/rc/clk?jk=e769bfff72e312be&amp;fccid=0e0b320a90f3822f&amp;vjs=3</t>
         </is>
       </c>
     </row>
     <row r="27">
-      <c r="B27" s="0" t="inlineStr"/>
-      <c r="C27" s="0" t="inlineStr"/>
-      <c r="D27" s="0" t="inlineStr"/>
+      <c r="A27" s="0" t="inlineStr">
+        <is>
+          <t>ASP.Net Developer</t>
+        </is>
+      </c>
+      <c r="B27" s="0" t="inlineStr">
+        <is>
+          <t>MicroVision</t>
+        </is>
+      </c>
+      <c r="C27" s="0" t="inlineStr">
+        <is>
+          <t>Dubai</t>
+        </is>
+      </c>
+      <c r="D27" s="0" t="inlineStr">
+        <is>
+          <t>Providing on-going support and development in ASP.Net.</t>
+        </is>
+      </c>
       <c r="E27" s="0" t="inlineStr">
         <is>
-          <t>Today</t>
+          <t>30+ days ago</t>
         </is>
       </c>
       <c r="F27" s="0" t="inlineStr">
         <is>
-          <t>https://ae.indeed.com/company/Resource-Log-LLC/jobs/PHP-Wordpress-Programmer-e5bf45b55a69d151?fccid=415cd241779a8615&amp;vjs=3</t>
+          <t>https://ae.indeed.com/rc/clk?jk=772e502b6378bb7e&amp;fccid=1e10041bb2747ae8&amp;vjs=3</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="0" t="inlineStr">
         <is>
-          <t>Web Developer</t>
-        </is>
-      </c>
-      <c r="B28" s="0" t="inlineStr"/>
-      <c r="C28" s="0" t="inlineStr"/>
-      <c r="D28" s="0" t="inlineStr"/>
+          <t>Waiter / Waitress</t>
+        </is>
+      </c>
+      <c r="B28" s="0" t="inlineStr">
+        <is>
+          <t>RBnH Solutions</t>
+        </is>
+      </c>
+      <c r="C28" s="0" t="inlineStr">
+        <is>
+          <t>Dubai</t>
+        </is>
+      </c>
+      <c r="D28" s="0" t="inlineStr">
+        <is>
+          <t>You will be a vital part in delivering an unrivaled customer experience on a daily basis.</t>
+        </is>
+      </c>
       <c r="E28" s="0" t="inlineStr">
         <is>
-          <t>30 days ago</t>
+          <t>6 days ago</t>
         </is>
       </c>
       <c r="F28" s="0" t="inlineStr">
         <is>
-          <t>https://ae.indeed.com/company/CENTURY-FINANCIAL/jobs/Web-Developer-30dac6d408ac0134?fccid=bcbae8ac47184d2d&amp;vjs=3</t>
+          <t>https://ae.indeed.com/rc/clk?jk=64bd894a16a530d6&amp;fccid=b7497ab89d75ef81&amp;vjs=3</t>
         </is>
       </c>
     </row>
     <row r="29">
-      <c r="B29" s="0" t="inlineStr"/>
-      <c r="C29" s="0" t="inlineStr"/>
-      <c r="D29" s="0" t="inlineStr"/>
+      <c r="A29" s="0" t="inlineStr">
+        <is>
+          <t>.NET Developer</t>
+        </is>
+      </c>
+      <c r="B29" s="0" t="inlineStr">
+        <is>
+          <t>Group Three IT Consultants</t>
+        </is>
+      </c>
+      <c r="C29" s="0" t="inlineStr">
+        <is>
+          <t>Dubai</t>
+        </is>
+      </c>
+      <c r="D29" s="0" t="inlineStr">
+        <is>
+          <t>NET developer who can build powerful desktop/web-based application using Microsoft .</t>
+        </is>
+      </c>
       <c r="E29" s="0" t="inlineStr">
         <is>
-          <t>2 days ago</t>
+          <t>30+ days ago</t>
         </is>
       </c>
       <c r="F29" s="0" t="inlineStr">
         <is>
-          <t>https://ae.indeed.com/company/OREX-Solar-Energy/jobs/IT-Web-Developer-baf02380a917c09a?fccid=2bee550ffb8b552a&amp;vjs=3</t>
+          <t>https://ae.indeed.com/rc/clk?jk=a966814adba1d4ae&amp;fccid=01fa4c4529403dd7&amp;vjs=3</t>
         </is>
       </c>
     </row>
     <row r="30">
-      <c r="B30" s="0" t="inlineStr"/>
-      <c r="C30" s="0" t="inlineStr"/>
-      <c r="D30" s="0" t="inlineStr"/>
+      <c r="A30" s="0" t="inlineStr">
+        <is>
+          <t>WEB DEVELOPER</t>
+        </is>
+      </c>
+      <c r="B30" s="0" t="inlineStr">
+        <is>
+          <t>Grow Combine</t>
+        </is>
+      </c>
+      <c r="C30" s="0" t="inlineStr">
+        <is>
+          <t>Dubai</t>
+        </is>
+      </c>
+      <c r="D30" s="0" t="inlineStr">
+        <is>
+          <t>Seeking web developers with extensive knowledge in designing, coding and modifying websites, from layout to function according to a client's specifications and…</t>
+        </is>
+      </c>
       <c r="E30" s="0" t="inlineStr">
         <is>
-          <t>2 days ago</t>
+          <t>30+ days ago</t>
         </is>
       </c>
       <c r="F30" s="0" t="inlineStr">
         <is>
-          <t>https://ae.indeed.com/company/Bidincars.com/jobs/Web-Developer-080a18e1cf14b035?fccid=4c8e0bec509a2141&amp;vjs=3</t>
+          <t>https://ae.indeed.com/rc/clk?jk=5d321abf7438d6e0&amp;fccid=01eb65a25f8a625a&amp;vjs=3</t>
         </is>
       </c>
     </row>
     <row r="31">
-      <c r="B31" s="0" t="inlineStr"/>
-      <c r="C31" s="0" t="inlineStr"/>
-      <c r="D31" s="0" t="inlineStr"/>
+      <c r="A31" s="0" t="inlineStr">
+        <is>
+          <t>Front-End Web Developer</t>
+        </is>
+      </c>
+      <c r="B31" s="0" t="inlineStr">
+        <is>
+          <t>Abbrevia</t>
+        </is>
+      </c>
+      <c r="C31" s="0" t="inlineStr">
+        <is>
+          <t>Dubai</t>
+        </is>
+      </c>
+      <c r="D31" s="0" t="inlineStr">
+        <is>
+          <t>Minimum 3 years of RELEVANT experience.</t>
+        </is>
+      </c>
       <c r="E31" s="0" t="inlineStr">
         <is>
-          <t>Today</t>
+          <t>30+ days ago</t>
         </is>
       </c>
       <c r="F31" s="0" t="inlineStr">
         <is>
-          <t>https://ae.indeed.com/company/Handelot-FZC/jobs/Senior-PHP-Developer-2b358e2d9d86d4bd?fccid=40ff66d173f37b67&amp;vjs=3</t>
+          <t>https://ae.indeed.com/rc/clk?jk=99676b641806bd1d&amp;fccid=69faf3b8ead09344&amp;vjs=3</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="0" t="inlineStr">
         <is>
-          <t>Senior Full Stack Developer</t>
-        </is>
-      </c>
-      <c r="B32" s="0" t="inlineStr"/>
-      <c r="C32" s="0" t="inlineStr"/>
-      <c r="D32" s="0" t="inlineStr"/>
+          <t>Team Leader, IT Quality Assurance</t>
+        </is>
+      </c>
+      <c r="B32" s="0" t="inlineStr">
+        <is>
+          <t>Commercial Bank of Dubai</t>
+        </is>
+      </c>
+      <c r="C32" s="0" t="inlineStr">
+        <is>
+          <t>Dubai</t>
+        </is>
+      </c>
+      <c r="D32" s="0" t="inlineStr">
+        <is>
+          <t>Create documentation to show issues which goes to the developers to resolve and re-testing as required.</t>
+        </is>
+      </c>
       <c r="E32" s="0" t="inlineStr">
         <is>
           <t>30+ days ago</t>
@@ -1103,69 +1409,127 @@
       </c>
       <c r="F32" s="0" t="inlineStr">
         <is>
-          <t>https://ae.indeed.com/company/Via-Dubai/jobs/Senior-Full-Stack-Developer-c3af3abddb9bdbf5?fccid=02c86010add331e5&amp;vjs=3</t>
+          <t>https://ae.indeed.com/rc/clk?jk=bb95d421e578aab3&amp;fccid=3eaa98a640f7774c&amp;vjs=3</t>
         </is>
       </c>
     </row>
     <row r="33">
-      <c r="B33" s="0" t="inlineStr"/>
-      <c r="C33" s="0" t="inlineStr"/>
-      <c r="D33" s="0" t="inlineStr"/>
+      <c r="A33" s="0" t="inlineStr">
+        <is>
+          <t>NODE JS Developer</t>
+        </is>
+      </c>
+      <c r="B33" s="0" t="inlineStr">
+        <is>
+          <t>BFL Group</t>
+        </is>
+      </c>
+      <c r="C33" s="0" t="inlineStr">
+        <is>
+          <t>Dubai</t>
+        </is>
+      </c>
+      <c r="D33" s="0" t="inlineStr">
+        <is>
+          <t>Participate in support activities to help UI developers integrate with RESTful services.</t>
+        </is>
+      </c>
       <c r="E33" s="0" t="inlineStr">
         <is>
-          <t>1 day ago</t>
+          <t>30+ days ago</t>
         </is>
       </c>
       <c r="F33" s="0" t="inlineStr">
         <is>
-          <t>https://ae.indeed.com/company/Rising-Hightech/jobs/Laravel-Developer-c80f5177499dec88?fccid=f0623874aa20f4b0&amp;vjs=3</t>
+          <t>https://ae.indeed.com/rc/clk?jk=42b6a03895bbb4dc&amp;fccid=c1762dfe22706976&amp;vjs=3</t>
         </is>
       </c>
     </row>
     <row r="34">
-      <c r="B34" s="0" t="inlineStr"/>
-      <c r="C34" s="0" t="inlineStr"/>
-      <c r="D34" s="0" t="inlineStr"/>
+      <c r="A34" s="0" t="inlineStr">
+        <is>
+          <t>Web Front-End Developer</t>
+        </is>
+      </c>
+      <c r="B34" s="0" t="inlineStr">
+        <is>
+          <t>Group Three IT Consultants</t>
+        </is>
+      </c>
+      <c r="C34" s="0" t="inlineStr">
+        <is>
+          <t>Dubai</t>
+        </is>
+      </c>
+      <c r="D34" s="0" t="inlineStr">
+        <is>
+          <t>HTML5, Javascript (plain + libraries), CSS3, and using them efficiently.</t>
+        </is>
+      </c>
       <c r="E34" s="0" t="inlineStr">
         <is>
-          <t>7 days ago</t>
+          <t>30+ days ago</t>
         </is>
       </c>
       <c r="F34" s="0" t="inlineStr">
         <is>
-          <t>https://ae.indeed.com/company/I-Book-Holiday/jobs/Senior-Web-Developer-496838da4ec02ad3?fccid=3c439dde7fdfa6c3&amp;vjs=3</t>
+          <t>https://ae.indeed.com/rc/clk?jk=46beea82aa17765d&amp;fccid=01fa4c4529403dd7&amp;vjs=3</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="0" t="inlineStr">
         <is>
-          <t>Full Stack Developer - Dubai - 6 Months</t>
-        </is>
-      </c>
-      <c r="B35" s="0" t="inlineStr"/>
-      <c r="C35" s="0" t="inlineStr"/>
-      <c r="D35" s="0" t="inlineStr"/>
+          <t>PHP Developer</t>
+        </is>
+      </c>
+      <c r="B35" s="0" t="inlineStr">
+        <is>
+          <t>ipix solutions</t>
+        </is>
+      </c>
+      <c r="C35" s="0" t="inlineStr">
+        <is>
+          <t>Dubai</t>
+        </is>
+      </c>
+      <c r="D35" s="0" t="inlineStr">
+        <is>
+          <t>Knowledge is a must), My SQL, MS SQL,Mongo DB,AWS,Agile ,Javascript,React .</t>
+        </is>
+      </c>
       <c r="E35" s="0" t="inlineStr">
         <is>
-          <t>30 days ago</t>
+          <t>30+ days ago</t>
         </is>
       </c>
       <c r="F35" s="0" t="inlineStr">
         <is>
-          <t>https://ae.indeed.com/company/P-L-M-E-SOFTWARE-HOUSE-LLC/jobs/Full-Stack-Developer-f1463998ed38a4c2?fccid=456913302166e579&amp;vjs=3</t>
+          <t>https://ae.indeed.com/rc/clk?jk=6dab182edd88b96f&amp;fccid=a4a6d84f02499146&amp;vjs=3</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="0" t="inlineStr">
         <is>
-          <t>Front End Developer</t>
-        </is>
-      </c>
-      <c r="B36" s="0" t="inlineStr"/>
-      <c r="C36" s="0" t="inlineStr"/>
-      <c r="D36" s="0" t="inlineStr"/>
+          <t>Sr. Microservices Developer</t>
+        </is>
+      </c>
+      <c r="B36" s="0" t="inlineStr">
+        <is>
+          <t>PIVOT technologies</t>
+        </is>
+      </c>
+      <c r="C36" s="0" t="inlineStr">
+        <is>
+          <t>Dubai</t>
+        </is>
+      </c>
+      <c r="D36" s="0" t="inlineStr">
+        <is>
+          <t>Minimum 5 years hands on experience designing and developing microservices using either Java/Spring Boot with Java 8/9.</t>
+        </is>
+      </c>
       <c r="E36" s="0" t="inlineStr">
         <is>
           <t>30+ days ago</t>
@@ -1173,42 +1537,167 @@
       </c>
       <c r="F36" s="0" t="inlineStr">
         <is>
-          <t>https://ae.indeed.com/company/Grand-Technology/jobs/Front-End-Developer-147c17f66cbf9f98?fccid=871778351f57c254&amp;vjs=3</t>
+          <t>https://ae.indeed.com/rc/clk?jk=455d95de7543b78a&amp;fccid=8c761ed5a3ba7e1b&amp;vjs=3</t>
         </is>
       </c>
     </row>
     <row r="37">
-      <c r="B37" s="0" t="inlineStr"/>
-      <c r="C37" s="0" t="inlineStr"/>
-      <c r="D37" s="0" t="inlineStr"/>
+      <c r="A37" s="0" t="inlineStr">
+        <is>
+          <t>SFCC - Front End Developer</t>
+        </is>
+      </c>
+      <c r="B37" s="0" t="inlineStr">
+        <is>
+          <t>Chalhoub Group</t>
+        </is>
+      </c>
+      <c r="C37" s="0" t="inlineStr">
+        <is>
+          <t>Dubai</t>
+        </is>
+      </c>
+      <c r="D37" s="0" t="inlineStr">
+        <is>
+          <t>Build cross-browser, cross-device compatible pages adhering to industry best practices.</t>
+        </is>
+      </c>
       <c r="E37" s="0" t="inlineStr">
         <is>
-          <t>7 days ago</t>
+          <t>30+ days ago</t>
         </is>
       </c>
       <c r="F37" s="0" t="inlineStr">
         <is>
-          <t>https://ae.indeed.com/company/28-LIGHTBULBS-Technologies/jobs/PHP-Wordpress-Developer-5e6e28d28daa9c95?fccid=c84d6205b9d4151d&amp;vjs=3</t>
+          <t>https://ae.indeed.com/rc/clk?jk=0aaf0c7e90db7879&amp;fccid=01f47b3f00b281a4&amp;vjs=3</t>
         </is>
       </c>
     </row>
     <row r="38">
-      <c r="A38" t="inlineStr">
-        <is>
-          <t>PHP Developer</t>
-        </is>
-      </c>
-      <c r="B38" t="inlineStr"/>
-      <c r="C38" t="inlineStr"/>
-      <c r="D38" t="inlineStr"/>
-      <c r="E38" t="inlineStr">
-        <is>
-          <t>30+ days ago</t>
-        </is>
-      </c>
-      <c r="F38" t="inlineStr">
-        <is>
-          <t>https://ae.indeed.com/company/First-WAP-International-DMCC/jobs/PHP-Developer-f2c8c317fd6384f5?fccid=855d99554d04415f&amp;vjs=3</t>
+      <c r="A38" s="0" t="inlineStr">
+        <is>
+          <t>Javascript Developer</t>
+        </is>
+      </c>
+      <c r="B38" s="0" t="inlineStr">
+        <is>
+          <t>Raqmiyat</t>
+        </is>
+      </c>
+      <c r="C38" s="0" t="inlineStr">
+        <is>
+          <t>Dubai</t>
+        </is>
+      </c>
+      <c r="D38" s="0" t="inlineStr">
+        <is>
+          <t>Responsibilities will include implementing visual elements and their behaviors with user interactions • You will work with both front-end and back-end web…</t>
+        </is>
+      </c>
+      <c r="E38" s="0" t="inlineStr">
+        <is>
+          <t>27 days ago</t>
+        </is>
+      </c>
+      <c r="F38" s="0" t="inlineStr">
+        <is>
+          <t>https://ae.indeed.com/rc/clk?jk=4d7c2222dc90f969&amp;fccid=7afa5fdaf37013fe&amp;vjs=3</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" s="0" t="inlineStr">
+        <is>
+          <t>ANDROID DEVELOPER</t>
+        </is>
+      </c>
+      <c r="B39" s="0" t="inlineStr">
+        <is>
+          <t>Grow Combine</t>
+        </is>
+      </c>
+      <c r="C39" s="0" t="inlineStr">
+        <is>
+          <t>Dubai</t>
+        </is>
+      </c>
+      <c r="D39" s="0" t="inlineStr">
+        <is>
+          <t>At Grow, we are in need of a Senior-level Android Developer to build out highly-viewed; impeccably-designed engaging Android applications and you have an…</t>
+        </is>
+      </c>
+      <c r="E39" s="0" t="inlineStr">
+        <is>
+          <t>30+ days ago</t>
+        </is>
+      </c>
+      <c r="F39" s="0" t="inlineStr">
+        <is>
+          <t>https://ae.indeed.com/rc/clk?jk=8b1c7e881897e048&amp;fccid=01eb65a25f8a625a&amp;vjs=3</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" s="0" t="inlineStr">
+        <is>
+          <t>ERP Developer</t>
+        </is>
+      </c>
+      <c r="B40" s="0" t="inlineStr">
+        <is>
+          <t>Kitopi</t>
+        </is>
+      </c>
+      <c r="C40" s="0" t="inlineStr">
+        <is>
+          <t>Dubai</t>
+        </is>
+      </c>
+      <c r="D40" s="0" t="inlineStr">
+        <is>
+          <t>As Kitopi’s Technical Developer, you will be confident consultative responsible for designing and implementing system solutions and be able to gather…</t>
+        </is>
+      </c>
+      <c r="E40" s="0" t="inlineStr">
+        <is>
+          <t>13 days ago</t>
+        </is>
+      </c>
+      <c r="F40" s="0" t="inlineStr">
+        <is>
+          <t>https://ae.indeed.com/rc/clk?jk=6bdfe9809531c802&amp;fccid=ed1f012bc9c5fc56&amp;vjs=3</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>Senior Front-end Developer</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>TenTwenty</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>Dubai</t>
+        </is>
+      </c>
+      <c r="D41" t="inlineStr">
+        <is>
+          <t>We are looking to fill a full-time position both on site and remote working is possible.</t>
+        </is>
+      </c>
+      <c r="E41" t="inlineStr">
+        <is>
+          <t>30+ days ago</t>
+        </is>
+      </c>
+      <c r="F41" t="inlineStr">
+        <is>
+          <t>https://ae.indeed.com/rc/clk?jk=7dd5bd76c065f8d3&amp;fccid=559e98f2d4dfbf56&amp;vjs=3</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
#30 rules added for filtering jobs based on provided post date
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -1,66 +1,38 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24131"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Freelance Project\job-scraper-backend\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{724B61C8-3CE8-4069-B6A2-3E239A91151E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20370" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="20370" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet" sheetId="1" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <definedNames/>
+  <calcPr calcId="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
-  <si>
-    <t>JobTitle</t>
-  </si>
-  <si>
-    <t>Company</t>
-  </si>
-  <si>
-    <t>Location</t>
-  </si>
-  <si>
-    <t>Summary</t>
-  </si>
-  <si>
-    <t>PostDate</t>
-  </si>
-  <si>
-    <t>JobUrl</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
+  <fonts count="2">
     <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
       <name val="Tahoma"/>
       <family val="2"/>
+      <color rgb="FF000000"/>
+      <sz val="10"/>
     </font>
     <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
       <name val="Tahoma"/>
       <family val="2"/>
+      <color rgb="FF000000"/>
+      <sz val="10"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -76,32 +48,91 @@
     </border>
   </borders>
   <cellStyleXfs count="5">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="5">
-    <cellStyle name="Heading" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
-    <cellStyle name="Heading1" xfId="2" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Result" xfId="3" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
-    <cellStyle name="Result2" xfId="4" xr:uid="{00000000-0005-0000-0000-000004000000}"/>
+    <cellStyle name="Heading" xfId="1"/>
+    <cellStyle name="Heading1" xfId="2"/>
+    <cellStyle name="Result" xfId="3"/>
+    <cellStyle name="Result2" xfId="4"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -389,33 +420,256 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:F11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" t="s">
-        <v>5</v>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>JobTitle</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>Company</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>Location</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>Summary</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>PostDate</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>JobUrl</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Back End Developer</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Dubai, United Arab Emirates</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>https://ae.linkedin.com/jobs/view/back-end-developer-at-aspire-technology-2649450278?refId=cbG1tl53SnUZEbHG9ONbGQ%3D%3D&amp;trackingId=%2BnwzUngfp1Zp70DAA2QCPQ%3D%3D&amp;position=1&amp;pageNum=0&amp;trk=public_jobs_jserp-result_search-card</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Full Stack Developer</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Dubai, United Arab Emirates</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>https://ae.linkedin.com/jobs/view/full-stack-developer-at-forefront-talent-2653706644?refId=cbG1tl53SnUZEbHG9ONbGQ%3D%3D&amp;trackingId=Y9VxnJ%2FmtIgQd%2BcX9LXj0Q%3D%3D&amp;position=2&amp;pageNum=0&amp;trk=public_jobs_jserp-result_search-card</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Back End Developer</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Dubai, United Arab Emirates</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>https://ae.linkedin.com/jobs/view/back-end-developer-at-stella-stays-2567470812?refId=cbG1tl53SnUZEbHG9ONbGQ%3D%3D&amp;trackingId=0x0s%2Bnz%2FTOGKDHjHnfbEdw%3D%3D&amp;position=3&amp;pageNum=0&amp;trk=public_jobs_jserp-result_search-card</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Web Developer</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>Dubai, Dubai, United Arab Emirates</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>3 days ago</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>https://ae.linkedin.com/jobs/view/web-developer-at-techcarrot-2652078433?refId=cbG1tl53SnUZEbHG9ONbGQ%3D%3D&amp;trackingId=jhB6AZw9fCdiFvSBpSMM9Q%3D%3D&amp;position=4&amp;pageNum=0&amp;trk=public_jobs_jserp-result_search-card</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Junior/Senior Software Engineer</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Dubai, United Arab Emirates</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>5 days ago</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>https://ae.linkedin.com/jobs/view/junior-senior-software-engineer-at-mackenzie-jones-middle-east-2641356427?refId=cbG1tl53SnUZEbHG9ONbGQ%3D%3D&amp;trackingId=rIc%2B4qvlYzW1JfDCnC4WIQ%3D%3D&amp;position=5&amp;pageNum=0&amp;trk=public_jobs_jserp-result_search-card</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>JUNIOR DEVELOPER - Dubai or Remote</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>Dubai, Dubai, United Arab Emirates</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>2 months ago</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>https://ae.linkedin.com/jobs/view/junior-developer-dubai-or-remote-at-cobblestone-energy-2616837676?refId=cbG1tl53SnUZEbHG9ONbGQ%3D%3D&amp;trackingId=M4oRO9369sADp9UcMOwdIA%3D%3D&amp;position=6&amp;pageNum=0&amp;trk=public_jobs_jserp-result_search-card</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Junior Developer</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>Dubai, United Arab Emirates</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>4 weeks ago</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>https://ae.linkedin.com/jobs/view/junior-developer-at-chalhoub-group-2609224500?refId=cbG1tl53SnUZEbHG9ONbGQ%3D%3D&amp;trackingId=UJI5wqyjIE2u7du2%2FAa6gQ%3D%3D&amp;position=7&amp;pageNum=0&amp;trk=public_jobs_jserp-result_search-card</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Blockchain Developer</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>Dubai, United Arab Emirates</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>1 week ago</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>https://ae.linkedin.com/jobs/view/blockchain-developer-at-vietne-2640551460?refId=cbG1tl53SnUZEbHG9ONbGQ%3D%3D&amp;trackingId=9FAMSnZS9s3DRxpanBylGA%3D%3D&amp;position=8&amp;pageNum=0&amp;trk=public_jobs_jserp-result_search-card</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Full Stack Engineer</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>Dubai, United Arab Emirates</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>3 weeks ago</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>https://ae.linkedin.com/jobs/view/full-stack-engineer-at-klanik-2606377905?refId=cbG1tl53SnUZEbHG9ONbGQ%3D%3D&amp;trackingId=N5lxZQte8zYZM%2B0ijjKnTQ%3D%3D&amp;position=9&amp;pageNum=0&amp;trk=public_jobs_jserp-result_search-card</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Back End Developer</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr"/>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>Dubai, United Arab Emirates</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr"/>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>2 weeks ago</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>https://ae.linkedin.com/jobs/view/back-end-developer-at-aspire-mena-2630813687?refId=cbG1tl53SnUZEbHG9ONbGQ%3D%3D&amp;trackingId=JLOeeqnuP3rRU%2F4vmZTd8g%3D%3D&amp;position=10&amp;pageNum=0&amp;trk=public_jobs_jserp-result_search-card</t>
+        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
#30 rename original results
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -1,12 +1,12 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="20370" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="0" fullCalcOnLoad="1"/>
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F11"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -468,207 +468,28 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Back End Developer</t>
+          <t>Backend Developer - Laravel</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Avrioc Technologies</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Dubai, United Arab Emirates</t>
+          <t>Abu Dhabi, UAE</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr"/>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>25 days ago</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>https://ae.linkedin.com/jobs/view/back-end-developer-at-aspire-technology-2649450278?refId=cbG1tl53SnUZEbHG9ONbGQ%3D%3D&amp;trackingId=%2BnwzUngfp1Zp70DAA2QCPQ%3D%3D&amp;position=1&amp;pageNum=0&amp;trk=public_jobs_jserp-result_search-card</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>Full Stack Developer</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>Dubai, United Arab Emirates</t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>https://ae.linkedin.com/jobs/view/full-stack-developer-at-forefront-talent-2653706644?refId=cbG1tl53SnUZEbHG9ONbGQ%3D%3D&amp;trackingId=Y9VxnJ%2FmtIgQd%2BcX9LXj0Q%3D%3D&amp;position=2&amp;pageNum=0&amp;trk=public_jobs_jserp-result_search-card</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>Back End Developer</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>Dubai, United Arab Emirates</t>
-        </is>
-      </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>https://ae.linkedin.com/jobs/view/back-end-developer-at-stella-stays-2567470812?refId=cbG1tl53SnUZEbHG9ONbGQ%3D%3D&amp;trackingId=0x0s%2Bnz%2FTOGKDHjHnfbEdw%3D%3D&amp;position=3&amp;pageNum=0&amp;trk=public_jobs_jserp-result_search-card</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>Web Developer</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>Dubai, Dubai, United Arab Emirates</t>
-        </is>
-      </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>3 days ago</t>
-        </is>
-      </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>https://ae.linkedin.com/jobs/view/web-developer-at-techcarrot-2652078433?refId=cbG1tl53SnUZEbHG9ONbGQ%3D%3D&amp;trackingId=jhB6AZw9fCdiFvSBpSMM9Q%3D%3D&amp;position=4&amp;pageNum=0&amp;trk=public_jobs_jserp-result_search-card</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>Junior/Senior Software Engineer</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>Dubai, United Arab Emirates</t>
-        </is>
-      </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>5 days ago</t>
-        </is>
-      </c>
-      <c r="F6" t="inlineStr">
-        <is>
-          <t>https://ae.linkedin.com/jobs/view/junior-senior-software-engineer-at-mackenzie-jones-middle-east-2641356427?refId=cbG1tl53SnUZEbHG9ONbGQ%3D%3D&amp;trackingId=rIc%2B4qvlYzW1JfDCnC4WIQ%3D%3D&amp;position=5&amp;pageNum=0&amp;trk=public_jobs_jserp-result_search-card</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>JUNIOR DEVELOPER - Dubai or Remote</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>Dubai, Dubai, United Arab Emirates</t>
-        </is>
-      </c>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>2 months ago</t>
-        </is>
-      </c>
-      <c r="F7" t="inlineStr">
-        <is>
-          <t>https://ae.linkedin.com/jobs/view/junior-developer-dubai-or-remote-at-cobblestone-energy-2616837676?refId=cbG1tl53SnUZEbHG9ONbGQ%3D%3D&amp;trackingId=M4oRO9369sADp9UcMOwdIA%3D%3D&amp;position=6&amp;pageNum=0&amp;trk=public_jobs_jserp-result_search-card</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>Junior Developer</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>Dubai, United Arab Emirates</t>
-        </is>
-      </c>
-      <c r="E8" t="inlineStr">
-        <is>
-          <t>4 weeks ago</t>
-        </is>
-      </c>
-      <c r="F8" t="inlineStr">
-        <is>
-          <t>https://ae.linkedin.com/jobs/view/junior-developer-at-chalhoub-group-2609224500?refId=cbG1tl53SnUZEbHG9ONbGQ%3D%3D&amp;trackingId=UJI5wqyjIE2u7du2%2FAa6gQ%3D%3D&amp;position=7&amp;pageNum=0&amp;trk=public_jobs_jserp-result_search-card</t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>Blockchain Developer</t>
-        </is>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>Dubai, United Arab Emirates</t>
-        </is>
-      </c>
-      <c r="E9" t="inlineStr">
-        <is>
-          <t>1 week ago</t>
-        </is>
-      </c>
-      <c r="F9" t="inlineStr">
-        <is>
-          <t>https://ae.linkedin.com/jobs/view/blockchain-developer-at-vietne-2640551460?refId=cbG1tl53SnUZEbHG9ONbGQ%3D%3D&amp;trackingId=9FAMSnZS9s3DRxpanBylGA%3D%3D&amp;position=8&amp;pageNum=0&amp;trk=public_jobs_jserp-result_search-card</t>
-        </is>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>Full Stack Engineer</t>
-        </is>
-      </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>Dubai, United Arab Emirates</t>
-        </is>
-      </c>
-      <c r="E10" t="inlineStr">
-        <is>
-          <t>3 weeks ago</t>
-        </is>
-      </c>
-      <c r="F10" t="inlineStr">
-        <is>
-          <t>https://ae.linkedin.com/jobs/view/full-stack-engineer-at-klanik-2606377905?refId=cbG1tl53SnUZEbHG9ONbGQ%3D%3D&amp;trackingId=N5lxZQte8zYZM%2B0ijjKnTQ%3D%3D&amp;position=9&amp;pageNum=0&amp;trk=public_jobs_jserp-result_search-card</t>
-        </is>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>Back End Developer</t>
-        </is>
-      </c>
-      <c r="B11" t="inlineStr"/>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>Dubai, United Arab Emirates</t>
-        </is>
-      </c>
-      <c r="D11" t="inlineStr"/>
-      <c r="E11" t="inlineStr">
-        <is>
-          <t>2 weeks ago</t>
-        </is>
-      </c>
-      <c r="F11" t="inlineStr">
-        <is>
-          <t>https://ae.linkedin.com/jobs/view/back-end-developer-at-aspire-mena-2630813687?refId=cbG1tl53SnUZEbHG9ONbGQ%3D%3D&amp;trackingId=JLOeeqnuP3rRU%2F4vmZTd8g%3D%3D&amp;position=10&amp;pageNum=0&amp;trk=public_jobs_jserp-result_search-card</t>
+          <t>https://www.gulftalent.com/uae/jobs/backend-developer-laravel-321947</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Linkedin location changed when uae
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:F25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -468,28 +468,495 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Backend Developer - Laravel</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>Avrioc Technologies</t>
+          <t>Project Manager</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Abu Dhabi, UAE</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr"/>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>25 days ago</t>
+          <t>Dubai, United Arab Emirates</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>https://www.gulftalent.com/uae/jobs/backend-developer-laravel-321947</t>
+          <t>https://ae.linkedin.com/jobs/view/project-manager-at-3db-events-2672870467?refId=cWmE%2B0M8h1r2qi3LmtQJtg%3D%3D&amp;trackingId=z%2FdQXLtwy9Ww%2BN9L6bEEiQ%3D%3D&amp;position=2&amp;pageNum=0&amp;trk=public_jobs_jserp-result_search-card</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Senior Project Manager</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Dubai, United Arab Emirates</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>7 days ago</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>https://ae.linkedin.com/jobs/view/senior-project-manager-at-mashreq-bank-2661664425?refId=cWmE%2B0M8h1r2qi3LmtQJtg%3D%3D&amp;trackingId=Vie%2FuJLL%2FOTybROPRC9Pqg%3D%3D&amp;position=3&amp;pageNum=0&amp;trk=public_jobs_jserp-result_search-card</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Project Manager</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Dubai, Dubai, United Arab Emirates</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>https://ae.linkedin.com/jobs/view/project-manager-at-sana-commerce-2672381177?refId=cWmE%2B0M8h1r2qi3LmtQJtg%3D%3D&amp;trackingId=ad9YZ53J04vbiwH5%2BUPXBA%3D%3D&amp;position=4&amp;pageNum=0&amp;trk=public_jobs_jserp-result_search-card</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Project Manager</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>Dubai, United Arab Emirates</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>3 days ago</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>https://ae.linkedin.com/jobs/view/project-manager-at-talents-uae-2669842845?refId=cWmE%2B0M8h1r2qi3LmtQJtg%3D%3D&amp;trackingId=Zdn5QfCkeRBY6CCIqD86RA%3D%3D&amp;position=5&amp;pageNum=0&amp;trk=public_jobs_jserp-result_search-card</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Project Manager</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Dubai, United Arab Emirates</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>1 week ago</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>https://ae.linkedin.com/jobs/view/project-manager-at-relience-ltd-2660025196?refId=cWmE%2B0M8h1r2qi3LmtQJtg%3D%3D&amp;trackingId=Mor8Owtv7tz7n2205JU0vw%3D%3D&amp;position=6&amp;pageNum=0&amp;trk=public_jobs_jserp-result_search-card</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Senior Project Manager</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>Dubai, Dubai, United Arab Emirates</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>https://ae.linkedin.com/jobs/view/senior-project-manager-at-turner-townsend-2667149378?refId=cWmE%2B0M8h1r2qi3LmtQJtg%3D%3D&amp;trackingId=nUSNuvGOhNG6uOdlY8DHig%3D%3D&amp;position=7&amp;pageNum=0&amp;trk=public_jobs_jserp-result_search-card</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Freelance Project Manager</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>Dubai, United Arab Emirates</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>2 days ago</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>https://ae.linkedin.com/jobs/view/freelance-project-manager-at-prolab-digital-llc-2667910346?refId=cWmE%2B0M8h1r2qi3LmtQJtg%3D%3D&amp;trackingId=Y%2Bhph4lhnfpCyrwCEkAkAQ%3D%3D&amp;position=8&amp;pageNum=0&amp;trk=public_jobs_jserp-result_search-card</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Project Manager</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>Dubai, United Arab Emirates</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>1 week ago</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>https://ae.linkedin.com/jobs/view/project-manager-at-sign-works-llc-2655714103?refId=cWmE%2B0M8h1r2qi3LmtQJtg%3D%3D&amp;trackingId=JuAtESQa7WwLycNHTTkHzw%3D%3D&amp;position=9&amp;pageNum=0&amp;trk=public_jobs_jserp-result_search-card</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Project Manager</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>Dubai, United Arab Emirates</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>4 weeks ago</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>https://ae.linkedin.com/jobs/view/project-manager-at-elsewedy-electric-2640119108?refId=cWmE%2B0M8h1r2qi3LmtQJtg%3D%3D&amp;trackingId=vViY37keANgTLM537puG%2Bg%3D%3D&amp;position=10&amp;pageNum=0&amp;trk=public_jobs_jserp-result_search-card</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Sr. Project Manager</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>Dubai, United Arab Emirates</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>4 weeks ago</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>https://ae.linkedin.com/jobs/view/sr-project-manager-at-epsilon-global-consulting-2629795302?refId=cWmE%2B0M8h1r2qi3LmtQJtg%3D%3D&amp;trackingId=tZ%2F%2BFxYntDPUtGcDMpV4Rg%3D%3D&amp;position=11&amp;pageNum=0&amp;trk=public_jobs_jserp-result_search-card</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>Project Manager - Fitout ( Talent Pool)</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>Dubai, United Arab Emirates</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>1 day ago</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>https://ae.linkedin.com/jobs/view/project-manager-fitout-talent-pool-at-al-tayer-group-2667969953?refId=cWmE%2B0M8h1r2qi3LmtQJtg%3D%3D&amp;trackingId=zBlXWKyUeegLp9aeUSgePw%3D%3D&amp;position=12&amp;pageNum=0&amp;trk=public_jobs_jserp-result_search-card</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>Brand Project Manager</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>Dubai, United Arab Emirates</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>3 weeks ago</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>https://ae.linkedin.com/jobs/view/brand-project-manager-at-noon-2644357673?refId=cWmE%2B0M8h1r2qi3LmtQJtg%3D%3D&amp;trackingId=ifezvT9WQ2zL%2B9ZRDnF%2Btw%3D%3D&amp;position=13&amp;pageNum=0&amp;trk=public_jobs_jserp-result_search-card</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>Project Manager - Pavilion (Expo)</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>Dubai, United Arab Emirates</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>https://ae.linkedin.com/jobs/view/project-manager-pavilion-expo-at-world-security-2668921191?refId=cWmE%2B0M8h1r2qi3LmtQJtg%3D%3D&amp;trackingId=rjKJp06bTArPYOeKUYGUAw%3D%3D&amp;position=14&amp;pageNum=0&amp;trk=public_jobs_jserp-result_search-card</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>Project Manager (Change &amp; Transformation) - 1 year contract</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>Dubai, United Arab Emirates</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>4 weeks ago</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>https://ae.linkedin.com/jobs/view/project-manager-change-transformation-1-year-contract-at-commercial-bank-international-2631901808?refId=cWmE%2B0M8h1r2qi3LmtQJtg%3D%3D&amp;trackingId=yutsJnY5Z%2BXKiLCdy4LYGw%3D%3D&amp;position=15&amp;pageNum=0&amp;trk=public_jobs_jserp-result_search-card</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>Head of Project Management</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>Dubai, Dubai, United Arab Emirates</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>1 week ago</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>https://ae.linkedin.com/jobs/view/head-of-project-management-at-encore-2656362283?refId=cWmE%2B0M8h1r2qi3LmtQJtg%3D%3D&amp;trackingId=cROBuarnmkEXbQw2KbGcvg%3D%3D&amp;position=16&amp;pageNum=0&amp;trk=public_jobs_jserp-result_search-card</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>Project Manager - 6 mths contract</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>Dubai, United Arab Emirates</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>1 week ago</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>https://ae.linkedin.com/jobs/view/project-manager-6-mths-contract-at-manpowergroup-middle-east-2662326668?refId=cWmE%2B0M8h1r2qi3LmtQJtg%3D%3D&amp;trackingId=TLfuvvRxY%2B9jAullaA%2B%2B4g%3D%3D&amp;position=17&amp;pageNum=0&amp;trk=public_jobs_jserp-result_search-card</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>Senior Project Manager</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>Dubai, United Arab Emirates</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>2 weeks ago</t>
+        </is>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>https://ae.linkedin.com/jobs/view/senior-project-manager-at-hantec-markets-2655474696?refId=cWmE%2B0M8h1r2qi3LmtQJtg%3D%3D&amp;trackingId=m1UsVaYW7r0%2BjyEXWiRWdw%3D%3D&amp;position=18&amp;pageNum=0&amp;trk=public_jobs_jserp-result_search-card</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>IT Manager - Projects / Events</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>Dubai, United Arab Emirates</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>3 days ago</t>
+        </is>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>https://ae.linkedin.com/jobs/view/it-manager-projects-events-at-falcon-and-associates-2667213702?refId=cWmE%2B0M8h1r2qi3LmtQJtg%3D%3D&amp;trackingId=Tu1UzYIXsjzh0aVjxSbpIg%3D%3D&amp;position=19&amp;pageNum=0&amp;trk=public_jobs_jserp-result_search-card</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>Innovation Project Manager</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>Dubai, United Arab Emirates</t>
+        </is>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>https://ae.linkedin.com/jobs/view/innovation-project-manager-at-dnata-2666301640?refId=cWmE%2B0M8h1r2qi3LmtQJtg%3D%3D&amp;trackingId=bgYKmmUumYFHJbS9Gi4dtw%3D%3D&amp;position=20&amp;pageNum=0&amp;trk=public_jobs_jserp-result_search-card</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>Technical Project Manager (Location-Based)</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>Dubai, Dubai, United Arab Emirates</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>2 weeks ago</t>
+        </is>
+      </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>https://ae.linkedin.com/jobs/view/technical-project-manager-location-based-at-magnopus-2655085650?refId=cWmE%2B0M8h1r2qi3LmtQJtg%3D%3D&amp;trackingId=7EN2M31T8kDc4Vu3WXV9RA%3D%3D&amp;position=21&amp;pageNum=0&amp;trk=public_jobs_jserp-result_search-card</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>Senior Project Manager - Hotels (FE-PM)</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>Dubai, United Arab Emirates</t>
+        </is>
+      </c>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>https://ae.linkedin.com/jobs/view/senior-project-manager-hotels-fe-pm-at-fifthedge-construction-recruitment-intelligence-2672670876?refId=cWmE%2B0M8h1r2qi3LmtQJtg%3D%3D&amp;trackingId=wMoWfNN0vSEq6hfYocyUEw%3D%3D&amp;position=22&amp;pageNum=0&amp;trk=public_jobs_jserp-result_search-card</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>Project Manager - IT</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>Dubai, Dubai, United Arab Emirates</t>
+        </is>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>1 month ago</t>
+        </is>
+      </c>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t>https://ae.linkedin.com/jobs/view/project-manager-it-at-majid-al-futtaim-2658682541?refId=cWmE%2B0M8h1r2qi3LmtQJtg%3D%3D&amp;trackingId=Ex5Y3Uv91M2XETYWeTJEsw%3D%3D&amp;position=23&amp;pageNum=0&amp;trk=public_jobs_jserp-result_search-card</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>Senior Manager, New Solutions</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>Dubai, Dubai, United Arab Emirates</t>
+        </is>
+      </c>
+      <c r="F24" t="inlineStr">
+        <is>
+          <t>https://ae.linkedin.com/jobs/view/senior-manager-new-solutions-at-visa-2666391375?refId=cWmE%2B0M8h1r2qi3LmtQJtg%3D%3D&amp;trackingId=zQrHnnvWj4x8fR1dxVQ5tA%3D%3D&amp;position=24&amp;pageNum=0&amp;trk=public_jobs_jserp-result_search-card</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>Project Manager</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr"/>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>Dubai, Dubai, United Arab Emirates</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr"/>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>6 days ago</t>
+        </is>
+      </c>
+      <c r="F25" t="inlineStr">
+        <is>
+          <t>https://ae.linkedin.com/jobs/view/project-manager-at-servion-global-solutions-2659556427?refId=cWmE%2B0M8h1r2qi3LmtQJtg%3D%3D&amp;trackingId=JibrnQFBhga8mRrgGoejyQ%3D%3D&amp;position=25&amp;pageNum=0&amp;trk=public_jobs_jserp-result_search-card</t>
         </is>
       </c>
     </row>

</xml_diff>